<commit_message>
Generate new gerber files
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -34,13 +34,25 @@
     <t xml:space="preserve">LCSC</t>
   </si>
   <si>
+    <t xml:space="preserve">R35, R36, R73, R74, R112, R113, R151, R152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R31, R32, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53, R54, R55, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R79, R80, R81, R82, R83, R84, R85, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R100, R101, R102, R103, R104, R105, R106, R107, R108, R118, R119, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R135, R136, R137, R138, R139, R140, R141, R142, R143, R144, R145, R146, R147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25091</t>
+  </si>
+  <si>
     <t xml:space="preserve">100k</t>
   </si>
   <si>
-    <t xml:space="preserve">R33, R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R0402</t>
+    <t xml:space="preserve">R33, R34, R70, R71, R109, R110, R148, R149</t>
   </si>
   <si>
     <t xml:space="preserve">C25741</t>
@@ -49,7 +61,7 @@
     <t xml:space="preserve">100nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C4, C5</t>
+    <t xml:space="preserve">C4, C5, C6, C7, C8, C17, C18, C19, C20, C21, C30, C31, C32, C33, C34, C43, C44, C45, C46, C47</t>
   </si>
   <si>
     <t xml:space="preserve">C0402K</t>
@@ -58,7 +70,7 @@
     <t xml:space="preserve">C1525</t>
   </si>
   <si>
-    <t xml:space="preserve">C6, C7, C8</t>
+    <t xml:space="preserve">R3, R72, R111, R150</t>
   </si>
   <si>
     <t xml:space="preserve">C52923</t>
@@ -67,7 +79,7 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
-    <t xml:space="preserve">R3</t>
+    <t xml:space="preserve">C2, C16, C29, C42</t>
   </si>
   <si>
     <t xml:space="preserve">C25744</t>
@@ -76,7 +88,7 @@
     <t xml:space="preserve">10uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C2</t>
+    <t xml:space="preserve">R38, R39, R77, R78, R116, R117, R155, R156</t>
   </si>
   <si>
     <t xml:space="preserve">CASE-A_3216</t>
@@ -85,52 +97,40 @@
     <t xml:space="preserve">C7171</t>
   </si>
   <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30, R76, R115, R154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11702</t>
+  </si>
+  <si>
     <t xml:space="preserve">1M</t>
   </si>
   <si>
-    <t xml:space="preserve">R30</t>
+    <t xml:space="preserve">C1, C14, C27, C40</t>
   </si>
   <si>
     <t xml:space="preserve">C26083</t>
   </si>
   <si>
-    <t xml:space="preserve">1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R38, R39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11702</t>
-  </si>
-  <si>
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R35, R36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4109</t>
+    <t xml:space="preserve">C9, C10, C11, C12, C22, C23, C24, C25, C35, C36, C37, C38, C48, C49, C50, C51</t>
   </si>
   <si>
     <t xml:space="preserve">20pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C9, C10, C11, C12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2, R4, R5, R6, R7, R8, R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R31, R32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25091</t>
+    <t xml:space="preserve">C3, C15, C28, C41</t>
   </si>
   <si>
     <t xml:space="preserve">22uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
+    <t xml:space="preserve">Q1, Q3, Q5, Q7</t>
   </si>
   <si>
     <t xml:space="preserve">CASE-R_2012</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">32.768kHz</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1</t>
+    <t xml:space="preserve">R37, R75, R114, R153</t>
   </si>
   <si>
     <t xml:space="preserve">SMD-3215_2P</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">4k7</t>
   </si>
   <si>
-    <t xml:space="preserve">R37</t>
+    <t xml:space="preserve">Q2, Q4, Q6, Q8</t>
   </si>
   <si>
     <t xml:space="preserve">C25900</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">8MHz</t>
   </si>
   <si>
-    <t xml:space="preserve">Q2</t>
+    <t xml:space="preserve">U2, U4, U6, U8</t>
   </si>
   <si>
     <t xml:space="preserve">SMD-5032_2P</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">AMS1117-3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">U2</t>
+    <t xml:space="preserve">C13, C26, C39, C52</t>
   </si>
   <si>
     <t xml:space="preserve">SOT-223</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">GREEN</t>
   </si>
   <si>
-    <t xml:space="preserve">C13</t>
+    <t xml:space="preserve">PWR, PWR1, PWR2, PWR3</t>
   </si>
   <si>
     <t xml:space="preserve">LED_0603</t>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">RED</t>
   </si>
   <si>
-    <t xml:space="preserve">PWR</t>
+    <t xml:space="preserve">U1, U3, U5, U7</t>
   </si>
   <si>
     <t xml:space="preserve">C2286</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">STM32F103C8T6</t>
   </si>
   <si>
-    <t xml:space="preserve">U1</t>
+    <t xml:space="preserve">U$1, U$2, U$3, U$4</t>
   </si>
   <si>
     <t xml:space="preserve">LQFP-48_7.0x7.0x0.5P</t>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t xml:space="preserve">TACTILE-SWITCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U$1</t>
   </si>
   <si>
     <t xml:space="preserve">SMD-SW-4_5.1x5.1x1.5</t>
@@ -241,6 +238,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -338,19 +336,19 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="121.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -363,142 +361,142 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="ALW1" s="0"/>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>30</v>
@@ -512,24 +510,24 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>220</v>
+      <c r="A12" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +566,7 @@
         <v>44</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>45</v>
@@ -649,13 +647,13 @@
         <v>65</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>